<commit_message>
Constant folding pass in semantic analyzer (#23)
</commit_message>
<xml_diff>
--- a/compiler/errors.xlsx
+++ b/compiler/errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afa/projects/HumanResourceCompiler/compiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C23B0A1-1D68-6343-9200-3C62C5367B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD0148E-3933-7F40-B452-588365DDF21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{2A65D4AE-18F2-5D4F-A247-5AA1CBFBFDAE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="25">
   <si>
     <t>Severity</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t xml:space="preserve">Expect a primary expression but got </t>
+  </si>
+  <si>
+    <t>Integer overflow (max 999 min -999)</t>
+  </si>
+  <si>
+    <t>Div 0/Mod0</t>
   </si>
 </sst>
 </file>
@@ -488,7 +494,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -807,6 +813,9 @@
       <c r="C15" t="s">
         <v>10</v>
       </c>
+      <c r="D15" t="s">
+        <v>23</v>
+      </c>
       <c r="E15">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C15,Stages!$A:$A,Stages!$B:$B)+$B15)</f>
         <v>3003</v>
@@ -825,6 +834,9 @@
       </c>
       <c r="C16" t="s">
         <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>24</v>
       </c>
       <c r="E16">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C16,Stages!$A:$A,Stages!$B:$B)+$B16)</f>

</xml_diff>

<commit_message>
Add check of variable use-before-initialization and variable shadowing (#24)
</commit_message>
<xml_diff>
--- a/compiler/errors.xlsx
+++ b/compiler/errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afa/projects/HumanResourceCompiler/compiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD0148E-3933-7F40-B452-588365DDF21D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12936E5-0F62-6F4C-8827-5CC2F1FF9DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{2A65D4AE-18F2-5D4F-A247-5AA1CBFBFDAE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="29">
   <si>
     <t>Severity</t>
   </si>
@@ -112,6 +112,18 @@
   </si>
   <si>
     <t>Div 0/Mod0</t>
+  </si>
+  <si>
+    <t>Subroutine signature mismatch</t>
+  </si>
+  <si>
+    <t>Warning</t>
+  </si>
+  <si>
+    <t>Variable shadows outer scope</t>
+  </si>
+  <si>
+    <t>Variable may be used before initialization</t>
   </si>
 </sst>
 </file>
@@ -161,7 +173,25 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -172,6 +202,25 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}" name="Table1" displayName="Table1" ref="A1:F28" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F28" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{C8BAA362-1C96-3A4B-A8C0-9A4361FE8517}" name="Severity"/>
+    <tableColumn id="2" xr3:uid="{ADEFBE20-AAE3-2B47-A872-E2F534480416}" name="ID"/>
+    <tableColumn id="3" xr3:uid="{1C98BB9C-A67F-CA4F-A948-E95BEA0AC752}" name="Stage"/>
+    <tableColumn id="4" xr3:uid="{E215C342-4709-3B45-8C5D-1A90D2B1FBCA}" name="Description"/>
+    <tableColumn id="5" xr3:uid="{E4E9CA02-8F6A-744C-89F5-FB48514CDB94}" name="ErrId">
+      <calculatedColumnFormula xml:space="preserve"> (_xlfn.XLOOKUP($C2,Stages!$A:$A,Stages!$B:$B)+$B2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{57AA14E7-673E-7446-83DE-9549ACFA454A}" name="FullId">
+      <calculatedColumnFormula xml:space="preserve"> LEFT(A2,1)&amp;E2</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,7 +543,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -857,6 +906,9 @@
       <c r="C17" t="s">
         <v>10</v>
       </c>
+      <c r="D17" t="s">
+        <v>25</v>
+      </c>
       <c r="E17">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C17,Stages!$A:$A,Stages!$B:$B)+$B17)</f>
         <v>3005</v>
@@ -868,13 +920,16 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>6</v>
       </c>
       <c r="C18" t="s">
         <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>27</v>
       </c>
       <c r="E18">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C18,Stages!$A:$A,Stages!$B:$B)+$B18)</f>
@@ -882,7 +937,7 @@
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>E3006</v>
+        <v>W3006</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -894,6 +949,9 @@
       </c>
       <c r="C19" t="s">
         <v>10</v>
+      </c>
+      <c r="D19" t="s">
+        <v>28</v>
       </c>
       <c r="E19">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C19,Stages!$A:$A,Stages!$B:$B)+$B19)</f>
@@ -1077,6 +1135,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add Dead Code Detection Pass in Semantic Analysis (#33)
- Added Dead Code Detection Pass
- Added Clear Symbol Table Pass and Remove Attribute Pass
- Allow remove attributes from ASTNode
- Reimplemented request-node-replacement in Semantic Analysis Visitor, and allow request-self-removal
- SemanticPassManager now supports adding symbol table
- Changed signature of `enter_node` to const ref to reduce copy costs
- Tests now supports `Expected: ` in comments to instruct output expectations
</commit_message>
<xml_diff>
--- a/compiler/errors.xlsx
+++ b/compiler/errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afa/projects/HumanResourceCompiler/compiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12936E5-0F62-6F4C-8827-5CC2F1FF9DB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62D8CF2-A4B0-0E41-A319-EBEAE95DDDEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{2A65D4AE-18F2-5D4F-A247-5AA1CBFBFDAE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
   <si>
     <t>Severity</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Variable may be used before initialization</t>
+  </si>
+  <si>
+    <t>Dead code</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -964,13 +967,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>8</v>
       </c>
       <c r="C20" t="s">
         <v>10</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
       </c>
       <c r="E20">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C20,Stages!$A:$A,Stages!$B:$B)+$B20)</f>
@@ -978,7 +984,7 @@
       </c>
       <c r="F20" t="str">
         <f t="shared" si="0"/>
-        <v>E3008</v>
+        <v>W3008</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add semantic analysis for unused variable (#47)
</commit_message>
<xml_diff>
--- a/compiler/errors.xlsx
+++ b/compiler/errors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afa/projects/HumanResourceCompiler/compiler/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\afa\projects\HumanResourceCompiler\compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D62D8CF2-A4B0-0E41-A319-EBEAE95DDDEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FE0D8C-2CDA-48B3-8D29-33E4531D86B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{2A65D4AE-18F2-5D4F-A247-5AA1CBFBFDAE}"/>
+    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{2A65D4AE-18F2-5D4F-A247-5AA1CBFBFDAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="36">
   <si>
     <t>Severity</t>
   </si>
@@ -127,6 +127,24 @@
   </si>
   <si>
     <t>Dead code</t>
+  </si>
+  <si>
+    <t>Invalid loop control statement context</t>
+  </si>
+  <si>
+    <t>Invalid return context</t>
+  </si>
+  <si>
+    <t>Not all path return a value</t>
+  </si>
+  <si>
+    <t>The function requires a return value but not given</t>
+  </si>
+  <si>
+    <t>The subprocedure cannot return a value but given</t>
+  </si>
+  <si>
+    <t>The variable is defined but not used</t>
   </si>
 </sst>
 </file>
@@ -546,16 +564,16 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -575,7 +593,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -597,7 +615,7 @@
         <v>E1001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -619,7 +637,7 @@
         <v>E2001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -641,7 +659,7 @@
         <v>E2002</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -663,7 +681,7 @@
         <v>E2003</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -685,7 +703,7 @@
         <v>E2004</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -707,7 +725,7 @@
         <v>E2005</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -729,7 +747,7 @@
         <v>E2006</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -751,7 +769,7 @@
         <v>E2007</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -773,7 +791,7 @@
         <v>E2008</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -792,7 +810,7 @@
         <v>E2009</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -811,7 +829,7 @@
         <v>E2010</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -833,7 +851,7 @@
         <v>E3001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -855,7 +873,7 @@
         <v>E3002</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -877,7 +895,7 @@
         <v>E3003</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -899,7 +917,7 @@
         <v>E3004</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -921,7 +939,7 @@
         <v>E3005</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>26</v>
       </c>
@@ -943,7 +961,7 @@
         <v>W3006</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -965,7 +983,7 @@
         <v>E3007</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -987,7 +1005,7 @@
         <v>W3008</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -996,6 +1014,9 @@
       </c>
       <c r="C21" t="s">
         <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>30</v>
       </c>
       <c r="E21">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C21,Stages!$A:$A,Stages!$B:$B)+$B21)</f>
@@ -1006,7 +1027,7 @@
         <v>E3009</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1015,6 +1036,9 @@
       </c>
       <c r="C22" t="s">
         <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
       </c>
       <c r="E22">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C22,Stages!$A:$A,Stages!$B:$B)+$B22)</f>
@@ -1025,7 +1049,7 @@
         <v>E3010</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1034,6 +1058,9 @@
       </c>
       <c r="C23" t="s">
         <v>10</v>
+      </c>
+      <c r="D23" t="s">
+        <v>32</v>
       </c>
       <c r="E23">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C23,Stages!$A:$A,Stages!$B:$B)+$B23)</f>
@@ -1044,7 +1071,7 @@
         <v>E3011</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1053,6 +1080,9 @@
       </c>
       <c r="C24" t="s">
         <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
       </c>
       <c r="E24">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C24,Stages!$A:$A,Stages!$B:$B)+$B24)</f>
@@ -1063,7 +1093,7 @@
         <v>E3012</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1072,6 +1102,9 @@
       </c>
       <c r="C25" t="s">
         <v>10</v>
+      </c>
+      <c r="D25" t="s">
+        <v>34</v>
       </c>
       <c r="E25">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C25,Stages!$A:$A,Stages!$B:$B)+$B25)</f>
@@ -1082,15 +1115,18 @@
         <v>E3013</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B26">
         <v>14</v>
       </c>
       <c r="C26" t="s">
         <v>10</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
       </c>
       <c r="E26">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C26,Stages!$A:$A,Stages!$B:$B)+$B26)</f>
@@ -1098,10 +1134,10 @@
       </c>
       <c r="F26" t="str">
         <f t="shared" si="0"/>
-        <v>E3014</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+        <v>W3014</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1120,7 +1156,7 @@
         <v>E3015</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1155,12 +1191,12 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1168,7 +1204,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1176,7 +1212,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1184,7 +1220,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1192,7 +1228,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
AST Interpreter and tests (#50)
</commit_message>
<xml_diff>
--- a/compiler/errors.xlsx
+++ b/compiler/errors.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\afa\projects\HumanResourceCompiler\compiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FE0D8C-2CDA-48B3-8D29-33E4531D86B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B316B7-E46A-4B55-9CB9-F6E44873F72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{2A65D4AE-18F2-5D4F-A247-5AA1CBFBFDAE}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
   <si>
     <t>Severity</t>
   </si>
@@ -145,6 +145,15 @@
   </si>
   <si>
     <t>The variable is defined but not used</t>
+  </si>
+  <si>
+    <t>Compiler</t>
+  </si>
+  <si>
+    <t>Interpreter</t>
+  </si>
+  <si>
+    <t>Accessed a null variable (unassigned)</t>
   </si>
 </sst>
 </file>
@@ -226,8 +235,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}" name="Table1" displayName="Table1" ref="A1:F28" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F28" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F29" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C8BAA362-1C96-3A4B-A8C0-9A4361FE8517}" name="Severity"/>
     <tableColumn id="2" xr3:uid="{ADEFBE20-AAE3-2B47-A872-E2F534480416}" name="ID"/>
@@ -561,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239B0A26-2073-5B4B-AB42-5A58C694B8C3}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -1175,6 +1184,28 @@
         <v>E3016</v>
       </c>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29">
+        <f xml:space="preserve"> (_xlfn.XLOOKUP($C29,Stages!$A:$A,Stages!$B:$B)+$B29)</f>
+        <v>69001</v>
+      </c>
+      <c r="F29" t="str">
+        <f xml:space="preserve"> LEFT(A29,1)&amp;E29</f>
+        <v>E69001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1185,10 +1216,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{012CEE78-3C2F-2D4A-B02C-6E38B0B89826}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -1236,6 +1267,22 @@
         <v>5000</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6">
+        <v>68000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7">
+        <v>69000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
IRGen: Add an SSA verifier pass to check SSA correctness
</commit_message>
<xml_diff>
--- a/compiler/errors.xlsx
+++ b/compiler/errors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\afa\projects\HumanResourceCompiler\compiler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afa/project/HumanResourceCompiler/compiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B316B7-E46A-4B55-9CB9-F6E44873F72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD98A91-6B62-A045-B256-30878AB71E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{2A65D4AE-18F2-5D4F-A247-5AA1CBFBFDAE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{2A65D4AE-18F2-5D4F-A247-5AA1CBFBFDAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
   <si>
     <t>Severity</t>
   </si>
@@ -72,9 +72,6 @@
     <t>SemAnalyzer</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>FullId</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>Accessed a null variable (unassigned)</t>
+  </si>
+  <si>
+    <t>IRGen</t>
   </si>
 </sst>
 </file>
@@ -235,8 +235,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F29" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}" name="Table1" displayName="Table1" ref="A1:F31" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F31" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C8BAA362-1C96-3A4B-A8C0-9A4361FE8517}" name="Severity"/>
     <tableColumn id="2" xr3:uid="{ADEFBE20-AAE3-2B47-A872-E2F534480416}" name="ID"/>
@@ -570,19 +570,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239B0A26-2073-5B4B-AB42-5A58C694B8C3}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,10 +599,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -624,7 +624,7 @@
         <v>E1001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -635,7 +635,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C3,Stages!$A:$A,Stages!$B:$B)+$B3)</f>
@@ -646,7 +646,7 @@
         <v>E2001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -657,7 +657,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C4,Stages!$A:$A,Stages!$B:$B)+$B4)</f>
@@ -668,7 +668,7 @@
         <v>E2002</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -679,7 +679,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C5,Stages!$A:$A,Stages!$B:$B)+$B5)</f>
@@ -690,7 +690,7 @@
         <v>E2003</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -701,7 +701,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C6,Stages!$A:$A,Stages!$B:$B)+$B6)</f>
@@ -712,7 +712,7 @@
         <v>E2004</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -723,7 +723,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C7,Stages!$A:$A,Stages!$B:$B)+$B7)</f>
@@ -734,7 +734,7 @@
         <v>E2005</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -745,7 +745,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C8,Stages!$A:$A,Stages!$B:$B)+$B8)</f>
@@ -756,7 +756,7 @@
         <v>E2006</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -767,7 +767,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C9,Stages!$A:$A,Stages!$B:$B)+$B9)</f>
@@ -778,7 +778,7 @@
         <v>E2007</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -789,7 +789,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C10,Stages!$A:$A,Stages!$B:$B)+$B10)</f>
@@ -800,7 +800,7 @@
         <v>E2008</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -819,7 +819,7 @@
         <v>E2009</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -838,7 +838,7 @@
         <v>E2010</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -849,7 +849,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C13,Stages!$A:$A,Stages!$B:$B)+$B13)</f>
@@ -860,7 +860,7 @@
         <v>E3001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -871,7 +871,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C14,Stages!$A:$A,Stages!$B:$B)+$B14)</f>
@@ -882,7 +882,7 @@
         <v>E3002</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -893,7 +893,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C15,Stages!$A:$A,Stages!$B:$B)+$B15)</f>
@@ -904,7 +904,7 @@
         <v>E3003</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -915,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C16,Stages!$A:$A,Stages!$B:$B)+$B16)</f>
@@ -926,7 +926,7 @@
         <v>E3004</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -937,7 +937,7 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C17,Stages!$A:$A,Stages!$B:$B)+$B17)</f>
@@ -948,18 +948,18 @@
         <v>E3005</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
         <v>26</v>
-      </c>
-      <c r="B18">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
       </c>
       <c r="E18">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C18,Stages!$A:$A,Stages!$B:$B)+$B18)</f>
@@ -970,7 +970,7 @@
         <v>W3006</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -981,7 +981,7 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C19,Stages!$A:$A,Stages!$B:$B)+$B19)</f>
@@ -992,9 +992,9 @@
         <v>E3007</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -1003,7 +1003,7 @@
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C20,Stages!$A:$A,Stages!$B:$B)+$B20)</f>
@@ -1014,7 +1014,7 @@
         <v>W3008</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C21,Stages!$A:$A,Stages!$B:$B)+$B21)</f>
@@ -1036,7 +1036,7 @@
         <v>E3009</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C22,Stages!$A:$A,Stages!$B:$B)+$B22)</f>
@@ -1058,7 +1058,7 @@
         <v>E3010</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C23,Stages!$A:$A,Stages!$B:$B)+$B23)</f>
@@ -1080,7 +1080,7 @@
         <v>E3011</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C24,Stages!$A:$A,Stages!$B:$B)+$B24)</f>
@@ -1102,7 +1102,7 @@
         <v>E3012</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C25,Stages!$A:$A,Stages!$B:$B)+$B25)</f>
@@ -1124,9 +1124,9 @@
         <v>E3013</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>14</v>
@@ -1135,7 +1135,7 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C26,Stages!$A:$A,Stages!$B:$B)+$B26)</f>
@@ -1146,7 +1146,7 @@
         <v>W3014</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>E3015</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>E3016</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1192,10 +1192,10 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" t="s">
         <v>37</v>
-      </c>
-      <c r="D29" t="s">
-        <v>38</v>
       </c>
       <c r="E29">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C29,Stages!$A:$A,Stages!$B:$B)+$B29)</f>
@@ -1204,6 +1204,44 @@
       <c r="F29" t="str">
         <f xml:space="preserve"> LEFT(A29,1)&amp;E29</f>
         <v>E69001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30">
+        <f xml:space="preserve"> (_xlfn.XLOOKUP($C30,Stages!$A:$A,Stages!$B:$B)+$B30)</f>
+        <v>5001</v>
+      </c>
+      <c r="F30" t="str">
+        <f xml:space="preserve"> LEFT(A30,1)&amp;E30</f>
+        <v>E5001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31">
+        <f xml:space="preserve"> (_xlfn.XLOOKUP($C31,Stages!$A:$A,Stages!$B:$B)+$B31)</f>
+        <v>5002</v>
+      </c>
+      <c r="F31" t="str">
+        <f xml:space="preserve"> LEFT(A31,1)&amp;E31</f>
+        <v>E5002</v>
       </c>
     </row>
   </sheetData>
@@ -1219,15 +1257,15 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1235,7 +1273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1243,7 +1281,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1251,7 +1289,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1259,25 +1297,25 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>68000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>69000</v>

</xml_diff>

<commit_message>
IRGen: Add an SSA verifier pass to check SSA correctness (#81)
</commit_message>
<xml_diff>
--- a/compiler/errors.xlsx
+++ b/compiler/errors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Debian\home\afa\projects\HumanResourceCompiler\compiler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afa/project/HumanResourceCompiler/compiler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B316B7-E46A-4B55-9CB9-F6E44873F72C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD98A91-6B62-A045-B256-30878AB71E30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32811" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{2A65D4AE-18F2-5D4F-A247-5AA1CBFBFDAE}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17260" xr2:uid="{2A65D4AE-18F2-5D4F-A247-5AA1CBFBFDAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
   <si>
     <t>Severity</t>
   </si>
@@ -72,9 +72,6 @@
     <t>SemAnalyzer</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
     <t>FullId</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>Accessed a null variable (unassigned)</t>
+  </si>
+  <si>
+    <t>IRGen</t>
   </si>
 </sst>
 </file>
@@ -235,8 +235,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}" name="Table1" displayName="Table1" ref="A1:F29" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A1:F29" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}" name="Table1" displayName="Table1" ref="A1:F31" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:F31" xr:uid="{BD2A3A12-51B0-9A4D-B304-869043A3B0A9}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{C8BAA362-1C96-3A4B-A8C0-9A4361FE8517}" name="Severity"/>
     <tableColumn id="2" xr3:uid="{ADEFBE20-AAE3-2B47-A872-E2F534480416}" name="ID"/>
@@ -570,19 +570,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{239B0A26-2073-5B4B-AB42-5A58C694B8C3}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="71.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -599,10 +599,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -624,7 +624,7 @@
         <v>E1001</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -635,7 +635,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C3,Stages!$A:$A,Stages!$B:$B)+$B3)</f>
@@ -646,7 +646,7 @@
         <v>E2001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -657,7 +657,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C4,Stages!$A:$A,Stages!$B:$B)+$B4)</f>
@@ -668,7 +668,7 @@
         <v>E2002</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -679,7 +679,7 @@
         <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E5">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C5,Stages!$A:$A,Stages!$B:$B)+$B5)</f>
@@ -690,7 +690,7 @@
         <v>E2003</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -701,7 +701,7 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C6,Stages!$A:$A,Stages!$B:$B)+$B6)</f>
@@ -712,7 +712,7 @@
         <v>E2004</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -723,7 +723,7 @@
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E7">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C7,Stages!$A:$A,Stages!$B:$B)+$B7)</f>
@@ -734,7 +734,7 @@
         <v>E2005</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -745,7 +745,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C8,Stages!$A:$A,Stages!$B:$B)+$B8)</f>
@@ -756,7 +756,7 @@
         <v>E2006</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -767,7 +767,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E9">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C9,Stages!$A:$A,Stages!$B:$B)+$B9)</f>
@@ -778,7 +778,7 @@
         <v>E2007</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -789,7 +789,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E10">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C10,Stages!$A:$A,Stages!$B:$B)+$B10)</f>
@@ -800,7 +800,7 @@
         <v>E2008</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -819,7 +819,7 @@
         <v>E2009</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -838,7 +838,7 @@
         <v>E2010</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>6</v>
       </c>
@@ -849,7 +849,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C13,Stages!$A:$A,Stages!$B:$B)+$B13)</f>
@@ -860,7 +860,7 @@
         <v>E3001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>6</v>
       </c>
@@ -871,7 +871,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C14,Stages!$A:$A,Stages!$B:$B)+$B14)</f>
@@ -882,7 +882,7 @@
         <v>E3002</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>6</v>
       </c>
@@ -893,7 +893,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E15">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C15,Stages!$A:$A,Stages!$B:$B)+$B15)</f>
@@ -904,7 +904,7 @@
         <v>E3003</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -915,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E16">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C16,Stages!$A:$A,Stages!$B:$B)+$B16)</f>
@@ -926,7 +926,7 @@
         <v>E3004</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -937,7 +937,7 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C17,Stages!$A:$A,Stages!$B:$B)+$B17)</f>
@@ -948,18 +948,18 @@
         <v>E3005</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
         <v>26</v>
-      </c>
-      <c r="B18">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D18" t="s">
-        <v>27</v>
       </c>
       <c r="E18">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C18,Stages!$A:$A,Stages!$B:$B)+$B18)</f>
@@ -970,7 +970,7 @@
         <v>W3006</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -981,7 +981,7 @@
         <v>10</v>
       </c>
       <c r="D19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E19">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C19,Stages!$A:$A,Stages!$B:$B)+$B19)</f>
@@ -992,9 +992,9 @@
         <v>E3007</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B20">
         <v>8</v>
@@ -1003,7 +1003,7 @@
         <v>10</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C20,Stages!$A:$A,Stages!$B:$B)+$B20)</f>
@@ -1014,7 +1014,7 @@
         <v>W3008</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -1025,7 +1025,7 @@
         <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E21">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C21,Stages!$A:$A,Stages!$B:$B)+$B21)</f>
@@ -1036,7 +1036,7 @@
         <v>E3009</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>10</v>
       </c>
       <c r="D22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C22,Stages!$A:$A,Stages!$B:$B)+$B22)</f>
@@ -1058,7 +1058,7 @@
         <v>E3010</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -1069,7 +1069,7 @@
         <v>10</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E23">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C23,Stages!$A:$A,Stages!$B:$B)+$B23)</f>
@@ -1080,7 +1080,7 @@
         <v>E3011</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>10</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E24">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C24,Stages!$A:$A,Stages!$B:$B)+$B24)</f>
@@ -1102,7 +1102,7 @@
         <v>E3012</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>10</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E25">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C25,Stages!$A:$A,Stages!$B:$B)+$B25)</f>
@@ -1124,9 +1124,9 @@
         <v>E3013</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26">
         <v>14</v>
@@ -1135,7 +1135,7 @@
         <v>10</v>
       </c>
       <c r="D26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E26">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C26,Stages!$A:$A,Stages!$B:$B)+$B26)</f>
@@ -1146,7 +1146,7 @@
         <v>W3014</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -1165,7 +1165,7 @@
         <v>E3015</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>E3016</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -1192,10 +1192,10 @@
         <v>1</v>
       </c>
       <c r="C29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" t="s">
         <v>37</v>
-      </c>
-      <c r="D29" t="s">
-        <v>38</v>
       </c>
       <c r="E29">
         <f xml:space="preserve"> (_xlfn.XLOOKUP($C29,Stages!$A:$A,Stages!$B:$B)+$B29)</f>
@@ -1204,6 +1204,44 @@
       <c r="F29" t="str">
         <f xml:space="preserve"> LEFT(A29,1)&amp;E29</f>
         <v>E69001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30">
+        <f xml:space="preserve"> (_xlfn.XLOOKUP($C30,Stages!$A:$A,Stages!$B:$B)+$B30)</f>
+        <v>5001</v>
+      </c>
+      <c r="F30" t="str">
+        <f xml:space="preserve"> LEFT(A30,1)&amp;E30</f>
+        <v>E5001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31">
+        <f xml:space="preserve"> (_xlfn.XLOOKUP($C31,Stages!$A:$A,Stages!$B:$B)+$B31)</f>
+        <v>5002</v>
+      </c>
+      <c r="F31" t="str">
+        <f xml:space="preserve"> LEFT(A31,1)&amp;E31</f>
+        <v>E5002</v>
       </c>
     </row>
   </sheetData>
@@ -1219,15 +1257,15 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1235,7 +1273,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1243,7 +1281,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1251,7 +1289,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1259,25 +1297,25 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6">
         <v>68000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>69000</v>

</xml_diff>